<commit_message>
Excel global e as minhas estatisticas(_Joao)
</commit_message>
<xml_diff>
--- a/stats_results/statistic_global.xlsx
+++ b/stats_results/statistic_global.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>config_DataSet1_Homog_Tournment2.txt</t>
   </si>
@@ -49,12 +49,6 @@
     <t>HOMOGENEO</t>
   </si>
   <si>
-    <t>RECOMBINATION</t>
-  </si>
-  <si>
-    <t>MUTATION</t>
-  </si>
-  <si>
     <t>SD</t>
   </si>
   <si>
@@ -80,32 +74,6 @@
   </si>
   <si>
     <t>CERCADA (µ)</t>
-  </si>
-  <si>
-    <r>
-      <t>FITNESS (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>FICHEIRO CONFIG.</t>
@@ -138,9 +106,6 @@
     <t>config_DataSet1_Random_Iteration10.txt</t>
   </si>
   <si>
-    <t>SELECTION</t>
-  </si>
-  <si>
     <t>FITNESS (µ)</t>
   </si>
   <si>
@@ -170,12 +135,45 @@
   <si>
     <t>1.6763054614240211</t>
   </si>
+  <si>
+    <t>config_DataSet1_Heterog_Iteration50.txt</t>
+  </si>
+  <si>
+    <t>config_DataSet1_Heterog_Iteration20.txt</t>
+  </si>
+  <si>
+    <t>config_DataSet1_Heterog_Iteration10.txt</t>
+  </si>
+  <si>
+    <t>HETEROGENEO</t>
+  </si>
+  <si>
+    <t>config_DataSet1_Heterog_Tournment2.txt</t>
+  </si>
+  <si>
+    <t>config_DataSet1_Heterog_Tournment3.txt</t>
+  </si>
+  <si>
+    <t>config_DataSet1_Heterog_Tournment4.txt</t>
+  </si>
+  <si>
+    <t>config_DataSet1_Heterog_Tournment5.txt</t>
+  </si>
+  <si>
+    <t>config_DataSet1_Heterog_Tournment6.txt</t>
+  </si>
+  <si>
+    <t>MUTAÇÃO (UNIFORM)</t>
+  </si>
+  <si>
+    <t>RECOMBINAÇÃO (ONE CUT)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,13 +188,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -234,9 +225,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -244,13 +234,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -308,12 +298,13 @@
             </a:r>
             <a:r>
               <a:rPr lang="pt-PT" baseline="0"/>
-              <a:t> do Torneio</a:t>
+              <a:t> do Torneio (Homogéneo)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -414,6 +405,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -550,6 +542,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -686,6 +679,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -810,6 +804,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -949,6 +944,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1051,7 +1047,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="pt-PT" baseline="0"/>
-              <a:t> das iterações</a:t>
+              <a:t> do Torneio (Heterogéneo)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
@@ -1099,7 +1095,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Iterations!$H$1</c:f>
+              <c:f>Tournment!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1178,76 +1174,56 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="9"/>
-              <c:pt idx="0">
-                <c:v>ADHOC 50</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>ADHOC 20</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>ADHOC 10</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>RND 50</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>RND 20</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>RND 10</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>HOMOG 50</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>HOMOG 20</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>HOMOG 10</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>Tournment!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Iterations!$H$2:$H$10</c:f>
+              <c:f>Tournment!$H$7:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.92</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.68</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.1500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8E0E-4A07-98B4-847B7B91E67F}"/>
+              <c16:uniqueId val="{00000000-5363-440D-B936-29FD89DC64F9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1256,7 +1232,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Iterations!$J$1</c:f>
+              <c:f>Tournment!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1335,76 +1311,56 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="9"/>
-              <c:pt idx="0">
-                <c:v>ADHOC 50</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>ADHOC 20</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>ADHOC 10</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>RND 50</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>RND 20</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>RND 10</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>HOMOG 50</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>HOMOG 20</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>HOMOG 10</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>Tournment!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Iterations!$J$2:$J$10</c:f>
+              <c:f>Tournment!$J$7:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>117.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>113.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>147.30000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3</c:v>
+                  <c:v>105.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.46</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.5</c:v>
+                  <c:v>116.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-8E0E-4A07-98B4-847B7B91E67F}"/>
+              <c16:uniqueId val="{00000001-5363-440D-B936-29FD89DC64F9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1413,7 +1369,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Iterations!$K$1</c:f>
+              <c:f>Tournment!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1492,76 +1448,56 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="9"/>
-              <c:pt idx="0">
-                <c:v>ADHOC 50</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>ADHOC 20</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>ADHOC 10</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>RND 50</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>RND 20</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>RND 10</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>HOMOG 50</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>HOMOG 20</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>HOMOG 10</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>Tournment!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Iterations!$K$2:$K$10</c:f>
+              <c:f>Tournment!$K$7:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>18.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>19.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.78</c:v>
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>19.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18.45</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18.8</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-8E0E-4A07-98B4-847B7B91E67F}"/>
+              <c16:uniqueId val="{00000002-5363-440D-B936-29FD89DC64F9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1576,11 +1512,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1866935727"/>
-        <c:axId val="1866946127"/>
+        <c:axId val="1865165343"/>
+        <c:axId val="1865159103"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1866935727"/>
+        <c:axId val="1865165343"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1607,8 +1543,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT"/>
-                  <a:t>Iterações</a:t>
+                  <a:t>Valor</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t> do torneio</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1679,7 +1620,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1866946127"/>
+        <c:crossAx val="1865159103"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1687,7 +1628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1866946127"/>
+        <c:axId val="1865159103"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,7 +1679,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1866935727"/>
+        <c:crossAx val="1865165343"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1792,10 +1733,847 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Variação das iterações</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.5454864769933263E-2"/>
+          <c:y val="0.21954301081226024"/>
+          <c:w val="0.96909027046013352"/>
+          <c:h val="0.59988792169255423"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Iterations!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FITNESS (µ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="12"/>
+              <c:pt idx="0">
+                <c:v>ADHOC 50</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>ADHOC 20</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>ADHOC 10</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>RND 50</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>RND 20</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>RND 10</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>HOMOG 50</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>HOMOG 20</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>HOMOG 10</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>HETEROG 50</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>HETEROG 20</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>HETEROG 10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Iterations!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8E0E-4A07-98B4-847B7B91E67F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Iterations!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CERCADA (µ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="12"/>
+              <c:pt idx="0">
+                <c:v>ADHOC 50</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>ADHOC 20</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>ADHOC 10</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>RND 50</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>RND 20</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>RND 10</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>HOMOG 50</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>HOMOG 20</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>HOMOG 10</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>HETEROG 50</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>HETEROG 20</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>HETEROG 10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Iterations!$J$2:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>162.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>168.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>140.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8E0E-4A07-98B4-847B7B91E67F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Iterations!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ITERAÇÕES (µ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="12"/>
+              <c:pt idx="0">
+                <c:v>ADHOC 50</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>ADHOC 20</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>ADHOC 10</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>RND 50</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>RND 20</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>RND 10</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>HOMOG 50</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>HOMOG 20</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>HOMOG 10</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>HETEROG 50</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>HETEROG 20</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>HETEROG 10</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Iterations!$K$2:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.739999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8E0E-4A07-98B4-847B7B91E67F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="1866935727"/>
+        <c:axId val="1866946127"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1866935727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Iterações</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46737967027040483"/>
+              <c:y val="0.93674057666865373"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1866946127"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1866946127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1866935727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1899,6 +2677,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2905,19 +3723,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2937,6 +4279,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2944,16 +4318,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2552699</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:colOff>914399</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3238,10 +4612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3259,73 +4633,73 @@
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>18</v>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>100</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>600</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.7</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0.1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="3">
         <v>20</v>
       </c>
     </row>
@@ -3333,34 +4707,34 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>100</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>600</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.7</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>3</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3">
         <v>4.7</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="3">
         <v>19.7</v>
       </c>
     </row>
@@ -3368,34 +4742,34 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>100</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>600</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.7</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>4</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>6.7</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3">
         <v>3.6</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>20</v>
       </c>
     </row>
@@ -3403,34 +4777,34 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>100</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>600</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.7</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.1</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>5</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>7.6</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>17</v>
       </c>
     </row>
@@ -3438,35 +4812,210 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>100</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>600</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.7</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>0.1</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>6</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>6</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3">
         <v>5.3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2">
+        <v>600</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>117.7</v>
+      </c>
+      <c r="K7" s="3">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2">
+        <v>100</v>
+      </c>
+      <c r="D8" s="2">
+        <v>600</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>113.1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="2">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2">
+        <v>600</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="K9" s="3">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2">
+        <v>100</v>
+      </c>
+      <c r="D10" s="2">
+        <v>600</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>105.4</v>
+      </c>
+      <c r="K10" s="3">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="2">
+        <v>100</v>
+      </c>
+      <c r="D11" s="2">
+        <v>600</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>116.7</v>
+      </c>
+      <c r="K11" s="3">
+        <v>19.5</v>
       </c>
     </row>
   </sheetData>
@@ -3478,11 +5027,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3490,367 +5037,473 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>18</v>
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="5">
-        <v>100</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1000</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>2</v>
-      </c>
-      <c r="H2" s="5">
-        <v>25</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="I2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3">
         <v>0</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3">
         <v>100</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>1000</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>0.7</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>0.1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>2</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>25</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="I3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="3">
         <v>0</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3">
         <v>100</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>1000</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>0.7</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>0.1</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>25</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="I4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3">
         <v>100</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>1000</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>0.7</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0.1</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>2.92</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="I5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3">
         <v>5.3</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>16.78</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3">
         <v>100</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>0.7</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>0.1</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>3.3</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="I6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="3">
         <v>4.8499999999999996</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>17.3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>100</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>1000</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>0.7</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>0.1</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>2</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>3.7</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="I7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="3">
         <v>4.5</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="3">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>100</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>1000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>0.7</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>0.1</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>2</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>4.68</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="I8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="3">
         <v>6.46</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <v>19.22</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>100</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>1000</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>0.7</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>0.1</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>2</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>4.1500000000000004</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="5">
+      <c r="I9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="3">
         <v>8.0500000000000007</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="3">
         <v>18.45</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>100</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>1000</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>0.7</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>0.1</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>4.3</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="I10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="3">
         <v>7.5</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="3">
         <v>18.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3">
+        <v>100</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>162.1</v>
+      </c>
+      <c r="K11" s="3">
+        <v>19.739999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="3">
+        <v>100</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>168.75</v>
+      </c>
+      <c r="K12" s="3">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>140.9</v>
+      </c>
+      <c r="K13" s="3">
+        <v>18.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>